<commit_message>
Added Update/Delete functions in device42 project
</commit_message>
<xml_diff>
--- a/Device42_project/csv_devices.xlsx
+++ b/Device42_project/csv_devices.xlsx
@@ -24,45 +24,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Network_Device</t>
-  </si>
-  <si>
-    <t>Blade_Chassis</t>
-  </si>
-  <si>
-    <t>Virtual_Host</t>
-  </si>
-  <si>
-    <t>In_Service</t>
-  </si>
-  <si>
-    <t>Service_Level</t>
-  </si>
-  <si>
-    <t>Serial_no</t>
-  </si>
-  <si>
-    <t>Asset_no</t>
-  </si>
-  <si>
-    <t>UUID</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>Blade_slot_no</t>
-  </si>
-  <si>
-    <t>Device_Host_Chassis</t>
-  </si>
-  <si>
     <t>TXARL1-MPC1</t>
   </si>
   <si>
@@ -199,6 +160,45 @@
   </si>
   <si>
     <t>34000803B9B30400000002C0</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>network_device</t>
+  </si>
+  <si>
+    <t>blade_chassis</t>
+  </si>
+  <si>
+    <t>virtual_host</t>
+  </si>
+  <si>
+    <t>in_service</t>
+  </si>
+  <si>
+    <t>service_level</t>
+  </si>
+  <si>
+    <t>serial_no</t>
+  </si>
+  <si>
+    <t>asset_no</t>
+  </si>
+  <si>
+    <t>uuid</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>blade_slot_no</t>
+  </si>
+  <si>
+    <t>device_host_chassis</t>
   </si>
 </sst>
 </file>
@@ -570,56 +570,59 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -627,10 +630,10 @@
         <v>288</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -645,19 +648,19 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="O2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -665,10 +668,10 @@
         <v>289</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -683,19 +686,19 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="L3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="O3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -703,10 +706,10 @@
         <v>290</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -721,16 +724,16 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="O4" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -738,10 +741,10 @@
         <v>291</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -756,19 +759,19 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="J5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="L5" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="O5" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -776,10 +779,10 @@
         <v>292</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -794,19 +797,19 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
         <v>16</v>
       </c>
-      <c r="I6" t="s">
-        <v>29</v>
-      </c>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="L6" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="O6" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -814,10 +817,10 @@
         <v>293</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
@@ -832,19 +835,19 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="L7" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="O7" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -852,10 +855,10 @@
         <v>294</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
@@ -870,19 +873,19 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="J8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="L8" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="O8" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -890,10 +893,10 @@
         <v>295</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -908,19 +911,19 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="I9" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="J9" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="L9" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="O9" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -928,10 +931,10 @@
         <v>296</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -946,19 +949,19 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="I10" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="J10" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="L10" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="O10" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -966,10 +969,10 @@
         <v>297</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -984,19 +987,19 @@
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="J11" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="L11" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="O11" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1004,37 +1007,37 @@
         <v>298</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" t="s">
         <v>36</v>
       </c>
-      <c r="D12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" t="s">
-        <v>49</v>
-      </c>
       <c r="J12" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="L12" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="O12" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1042,10 +1045,10 @@
         <v>299</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -1060,19 +1063,19 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="I13" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="J13" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="L13" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="O13" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1080,10 +1083,10 @@
         <v>300</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -1098,19 +1101,19 @@
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="I14" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="J14" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="L14" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="O14" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1118,10 +1121,10 @@
         <v>301</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -1136,19 +1139,19 @@
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="I15" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="J15" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="L15" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="O15" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>